<commit_message>
updated refr water temps
</commit_message>
<xml_diff>
--- a/HeatXCalculations.xlsx
+++ b/HeatXCalculations.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akullman\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a97Dr\OneDrive\Documents\College\CHEME_485\TeamA6\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_9966B606CD35508A196FBBCFB91F160E1F4092B1" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FA92CEE-1B9D-4B4F-84E6-F085F76AD911}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20483" windowHeight="7305"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -119,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,21 +439,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="15.265625" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.3984375" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G1" t="s">
         <v>0</v>
       </c>
@@ -461,12 +470,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>-62</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -489,19 +498,19 @@
       </c>
       <c r="J2">
         <f>((I2-B2)-(I2-B3))/LN((I2-B2)/(I2-B3))</f>
-        <v>22.680461522249502</v>
+        <v>80.796203954584584</v>
       </c>
       <c r="K2">
         <f>H2/(B6*J2)</f>
-        <v>6.2070121443159874</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+        <v>18.512815150087583</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>-35</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -528,10 +537,10 @@
       </c>
       <c r="K3">
         <f>H3/(B7*J3)</f>
-        <v>1.0234067971868421</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+        <v>14.583546859912499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -563,10 +572,10 @@
       </c>
       <c r="K4">
         <f>H4/(J4*B6)</f>
-        <v>8.755006974577622</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <v>93.021949104887227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -598,15 +607,15 @@
       </c>
       <c r="K5">
         <f>H5/(B7*J5)</f>
-        <v>2.6406748376913685</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+        <v>37.629616437102001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>850</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -616,12 +625,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1140</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -648,7 +657,7 @@
         <v>53.16882127204596</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -677,7 +686,7 @@
         <v>53.633186880551634</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -705,7 +714,7 @@
         <v>9.5643238111148765</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -717,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>

</xml_diff>